<commit_message>
Add formatted Excel workbook
</commit_message>
<xml_diff>
--- a/CognitiveImpairment/Output/metaAnalysisCognitiveImpairment-domainEstimates.xlsx
+++ b/CognitiveImpairment/Output/metaAnalysisCognitiveImpairment-domainEstimates.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
+    <t>is5FU</t>
+  </si>
+  <si>
     <t>domain</t>
-  </si>
-  <si>
-    <t>is5FU</t>
   </si>
   <si>
     <t>estimate</t>
@@ -208,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +386,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -549,9 +555,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -633,11 +640,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H17" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:H17"/>
   <sortState ref="A2:H17">
-    <sortCondition ref="A1:A17"/>
+    <sortCondition ref="B1:B17"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="domain"/>
-    <tableColumn id="2" name="is5FU"/>
+    <tableColumn id="1" name="is5FU"/>
+    <tableColumn id="2" name="domain"/>
     <tableColumn id="3" name="estimate" dataDxfId="6"/>
     <tableColumn id="4" name="se" dataDxfId="5"/>
     <tableColumn id="5" name="zval" dataDxfId="4"/>
@@ -939,13 +946,13 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="A1:H17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -980,11 +987,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>-0.14127813872242301</v>
@@ -1006,37 +1013,37 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
       <c r="C3" s="1">
-        <v>0.26235252428657402</v>
+        <v>0.121074385563978</v>
       </c>
       <c r="D3" s="1">
-        <v>0.22305018561684101</v>
+        <v>0.148810734798101</v>
       </c>
       <c r="E3" s="1">
-        <v>1.176204016872</v>
+        <v>0.81361324993285</v>
       </c>
       <c r="F3" s="1">
-        <v>0.239513359727129</v>
+        <v>0.41586654492452801</v>
       </c>
       <c r="G3" s="1">
-        <v>-0.174817806267409</v>
+        <v>-0.17058929515324001</v>
       </c>
       <c r="H3" s="1">
-        <v>0.69952285484055698</v>
+        <v>0.41273806628119702</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="b">
-        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0.192461839673192</v>
@@ -1058,37 +1065,37 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
       <c r="C5" s="1">
-        <v>-0.428340334137853</v>
+        <v>2.6474029820603699E-2</v>
       </c>
       <c r="D5" s="1">
-        <v>0.43837772442429401</v>
+        <v>0.17395967784973099</v>
       </c>
       <c r="E5" s="1">
-        <v>-0.97710332955529999</v>
+        <v>0.15218486345710799</v>
       </c>
       <c r="F5" s="1">
-        <v>0.328517999573123</v>
+        <v>0.87904113211504598</v>
       </c>
       <c r="G5" s="1">
-        <v>-1.2875448856340901</v>
+        <v>-0.314480673527058</v>
       </c>
       <c r="H5" s="1">
-        <v>0.43086421735838698</v>
+        <v>0.36742873316826602</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="b">
-        <v>0</v>
       </c>
       <c r="C6" s="1">
         <v>0.15737436034954699</v>
@@ -1110,37 +1117,37 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
       <c r="C7" s="1">
-        <v>-0.36205548612361799</v>
+        <v>5.7671398513899699E-2</v>
       </c>
       <c r="D7" s="1">
-        <v>0.44461013222171802</v>
+        <v>0.20640564412595</v>
       </c>
       <c r="E7" s="1">
-        <v>-0.81432126684658701</v>
+        <v>0.27940804990152401</v>
       </c>
       <c r="F7" s="1">
-        <v>0.41546092958362202</v>
+        <v>0.77993169406570095</v>
       </c>
       <c r="G7" s="1">
-        <v>-1.23347533243978</v>
+        <v>-0.34687623017875402</v>
       </c>
       <c r="H7" s="1">
-        <v>0.50936436019254105</v>
+        <v>0.462219027206554</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" t="b">
-        <v>0</v>
       </c>
       <c r="C8" s="1">
         <v>-0.36588113142102902</v>
@@ -1162,37 +1169,37 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
       <c r="C9" s="1">
-        <v>2.2538475341870399E-2</v>
+        <v>-8.0990131792208403E-2</v>
       </c>
       <c r="D9" s="1">
-        <v>0.89271702758639304</v>
+        <v>0.22781462082584</v>
       </c>
       <c r="E9" s="1">
-        <v>2.52470543804982E-2</v>
+        <v>-0.35550892870095502</v>
       </c>
       <c r="F9" s="1">
-        <v>0.97985790493485303</v>
+        <v>0.72220835710266096</v>
       </c>
       <c r="G9" s="1">
-        <v>-1.7271547471131099</v>
+        <v>-0.52749858376250203</v>
       </c>
       <c r="H9" s="1">
-        <v>1.77223169779685</v>
+        <v>0.365518320178086</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" t="b">
-        <v>0</v>
       </c>
       <c r="C10" s="1">
         <v>0.30640565553756</v>
@@ -1214,37 +1221,37 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
       <c r="C11" s="1">
-        <v>-0.37382786151646602</v>
+        <v>0.19493031830982999</v>
       </c>
       <c r="D11" s="1">
-        <v>0.69468013178535704</v>
+        <v>0.26240086608756802</v>
       </c>
       <c r="E11" s="1">
-        <v>-0.53812948494109503</v>
+        <v>0.74287223672797797</v>
       </c>
       <c r="F11" s="1">
-        <v>0.59048765791407898</v>
+        <v>0.457559035857244</v>
       </c>
       <c r="G11" s="1">
-        <v>-1.7353759005913001</v>
+        <v>-0.31936592873392</v>
       </c>
       <c r="H11" s="1">
-        <v>0.98772017755837105</v>
+        <v>0.70922656535358097</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" t="b">
-        <v>0</v>
       </c>
       <c r="C12" s="1">
         <v>1.4064807177746199</v>
@@ -1266,37 +1273,37 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="b">
-        <v>1</v>
-      </c>
       <c r="C13" s="1">
-        <v>-1.84501870242584</v>
+        <v>-0.176185460372766</v>
       </c>
       <c r="D13" s="1">
-        <v>0.35642908029508702</v>
+        <v>0.14869625006656301</v>
       </c>
       <c r="E13" s="1">
-        <v>-5.1763977868987503</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2.26210889605947E-7</v>
+        <v>-1.1848682148601399</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.23606955639827301</v>
       </c>
       <c r="G13" s="1">
-        <v>-2.5436068628469499</v>
+        <v>-0.467624755139391</v>
       </c>
       <c r="H13" s="1">
-        <v>-1.14643054200474</v>
+        <v>0.115253834393859</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" t="b">
-        <v>0</v>
       </c>
       <c r="C14" s="1">
         <v>1.01384561099315</v>
@@ -1318,37 +1325,37 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="b">
-        <v>1</v>
-      </c>
       <c r="C15" s="1">
-        <v>-1.0361547467415999</v>
+        <v>0.24004338853923801</v>
       </c>
       <c r="D15" s="1">
-        <v>0.397845632909618</v>
+        <v>0.17312870543255199</v>
       </c>
       <c r="E15" s="1">
-        <v>-2.6044140265251801</v>
-      </c>
-      <c r="F15" s="1">
-        <v>9.2031507142334903E-3</v>
+        <v>1.38650253254943</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.16559350749466101</v>
       </c>
       <c r="G15" s="1">
-        <v>-1.8159178586509901</v>
+        <v>-9.9282638798608505E-2</v>
       </c>
       <c r="H15" s="1">
-        <v>-0.25639163483220301</v>
+        <v>0.57936941587708501</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
-      </c>
-      <c r="B16" t="b">
-        <v>0</v>
       </c>
       <c r="C16" s="1">
         <v>-0.36450330833809702</v>
@@ -1370,29 +1377,29 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="b">
-        <v>1</v>
-      </c>
       <c r="C17" s="1">
-        <v>0.53105088878935203</v>
+        <v>0.428900104737861</v>
       </c>
       <c r="D17" s="1">
-        <v>2.7209226922639802</v>
+        <v>0.63320146523395304</v>
       </c>
       <c r="E17" s="1">
-        <v>0.195173089738718</v>
+        <v>0.67735172498280904</v>
       </c>
       <c r="F17" s="1">
-        <v>0.84525744520847201</v>
+        <v>0.49818281988594099</v>
       </c>
       <c r="G17" s="1">
-        <v>-4.8018595927658199</v>
+        <v>-0.81215196207867901</v>
       </c>
       <c r="H17" s="1">
-        <v>5.8639613703445201</v>
+        <v>1.6699521715543999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>